<commit_message>
Clean up before adding Readme section to git
</commit_message>
<xml_diff>
--- a/Kinematic/Doc/Calculation.xlsx
+++ b/Kinematic/Doc/Calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weifeng Huang\Desktop\MCKRobot\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weifeng Huang\Desktop\MCKRobot\Kinematic\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EBAC96-D50F-4765-9F0D-D8A9C1C81880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469BF00C-58DA-4894-8BBA-34053748CF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7725" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -500,7 +500,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,11 +591,11 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>234</v>
+        <v>550</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C16" si="0">B3/1000*9.8</f>
-        <v>2.2932000000000001</v>
+        <v>5.3900000000000006</v>
       </c>
       <c r="D3">
         <v>420</v>
@@ -609,7 +609,7 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G16" si="2">C3*E3*F3</f>
-        <v>0.963144</v>
+        <v>2.2638000000000003</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H11" si="3">D3-200</f>
@@ -621,7 +621,7 @@
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J11" si="5">F3*C3*I3</f>
-        <v>0.50450400000000006</v>
+        <v>1.1858000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -743,11 +743,11 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>327</v>
+        <v>550</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>3.2046000000000006</v>
+        <v>5.3900000000000006</v>
       </c>
       <c r="D7">
         <v>380</v>
@@ -761,7 +761,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>1.2177480000000003</v>
+        <v>2.0482</v>
       </c>
       <c r="H7">
         <f t="shared" si="3"/>
@@ -773,7 +773,7 @@
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
-        <v>0.57682800000000012</v>
+        <v>0.97020000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -933,11 +933,11 @@
         <v>23</v>
       </c>
       <c r="B12">
-        <v>231</v>
+        <v>550</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>2.2638000000000003</v>
+        <v>5.3900000000000006</v>
       </c>
       <c r="D12">
         <v>210</v>
@@ -951,7 +951,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>0.47539800000000004</v>
+        <v>1.1319000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1037,11 +1037,11 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>327</v>
+        <v>550</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>3.2046000000000006</v>
+        <v>5.3900000000000006</v>
       </c>
       <c r="D16">
         <v>160</v>
@@ -1055,17 +1055,17 @@
       </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>0.51273600000000008</v>
+        <v>0.86240000000000006</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G17">
         <f>SUM(G2:G16)</f>
-        <v>7.308644000000001</v>
+        <v>10.445917999999999</v>
       </c>
       <c r="J17">
         <f>SUM(J2:J16)</f>
-        <v>2.3605260000000006</v>
+        <v>3.4351940000000005</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1084,7 +1084,7 @@
         <v>43</v>
       </c>
       <c r="B19">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="C19">
         <f>160/12</f>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="G19">
         <f>B19*C19*D19</f>
-        <v>10.666666666666668</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>